<commit_message>
modificacion del modelo Task
</commit_message>
<xml_diff>
--- a/seeders/Table_Budget.xlsx
+++ b/seeders/Table_Budget.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GitHub\do-and-check_back\seeders\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GitHub\do_and_check_back2\seeders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE323ACD-0A5A-40B4-B882-C6344D0C40C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F5A1B4-AA67-489B-B730-C0A338697463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{78331709-7AEC-4852-8807-FA6C03489801}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="55">
   <si>
     <t>code</t>
   </si>
@@ -201,17 +201,21 @@
   </si>
   <si>
     <t>totalLabourCost</t>
-  </si>
-  <si>
-    <t>budgetPerfRatio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -246,59 +250,12 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -308,21 +265,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -445,6 +387,51 @@
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -459,19 +446,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{73859FA6-B201-4B3E-AA95-B0103745529F}" name="Tabla1" displayName="Tabla1" ref="A1:J38" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:J38" xr:uid="{73859FA6-B201-4B3E-AA95-B0103745529F}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{02AB9CA0-F38A-4F84-B089-91407259440B}" name="code" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{28BAAC49-883E-4794-B5A9-A36102880638}" name="title" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{45D60C40-648C-4915-8246-855E6240C002}" name="description" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{1A487E48-40EA-4B23-A821-233B479E0007}" name="taskGroup" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{50E1C117-0C18-4F8C-8E11-8574C6A6DF81}" name="taskStatus" dataDxfId="0"/>
-    <tableColumn id="6" xr3:uid="{604AAADE-9C9E-4848-AD83-955E0F214682}" name="unit" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{0C826A12-79CF-4C51-AE86-631B484247B9}" name="totalBudgetQty" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{292D0ECB-729B-472C-B2BB-C538B430EE2E}" name="totalBudgetHrs" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{42B9CA9F-909E-4799-B73A-EE7BE06E26CD}" name="totalLabourCost" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{9DB1281E-7DF4-48AF-BC5D-09FAF14D1045}" name="budgetPerfRatio" dataDxfId="4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{73859FA6-B201-4B3E-AA95-B0103745529F}" name="Tabla1" displayName="Tabla1" ref="A1:I38" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:I38" xr:uid="{73859FA6-B201-4B3E-AA95-B0103745529F}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{02AB9CA0-F38A-4F84-B089-91407259440B}" name="code" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{28BAAC49-883E-4794-B5A9-A36102880638}" name="title" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{45D60C40-648C-4915-8246-855E6240C002}" name="description" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{1A487E48-40EA-4B23-A821-233B479E0007}" name="taskGroup" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{50E1C117-0C18-4F8C-8E11-8574C6A6DF81}" name="taskStatus" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{604AAADE-9C9E-4848-AD83-955E0F214682}" name="unit" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{0C826A12-79CF-4C51-AE86-631B484247B9}" name="totalBudgetQty" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{292D0ECB-729B-472C-B2BB-C538B430EE2E}" name="totalBudgetHrs" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{42B9CA9F-909E-4799-B73A-EE7BE06E26CD}" name="totalLabourCost" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -777,7 +763,7 @@
   <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -825,9 +811,7 @@
       <c r="I1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>55</v>
-      </c>
+      <c r="J1"/>
       <c r="K1"/>
       <c r="L1"/>
       <c r="M1"/>
@@ -843,7 +827,7 @@
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -858,9 +842,7 @@
       <c r="I2" s="2">
         <v>126.31578947368421</v>
       </c>
-      <c r="J2" s="1">
-        <v>0.21</v>
-      </c>
+      <c r="J2"/>
       <c r="K2"/>
       <c r="L2"/>
       <c r="M2"/>
@@ -876,7 +858,7 @@
       <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -891,9 +873,7 @@
       <c r="I3" s="2">
         <v>252.63157894736841</v>
       </c>
-      <c r="J3" s="1">
-        <v>0.21</v>
-      </c>
+      <c r="J3"/>
       <c r="K3"/>
       <c r="L3"/>
       <c r="M3"/>
@@ -909,7 +889,7 @@
       <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -924,9 +904,7 @@
       <c r="I4" s="2">
         <v>400</v>
       </c>
-      <c r="J4" s="1">
-        <v>0.31</v>
-      </c>
+      <c r="J4"/>
       <c r="K4"/>
       <c r="L4"/>
       <c r="M4"/>
@@ -942,7 +920,7 @@
       <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -957,9 +935,7 @@
       <c r="I5" s="2">
         <v>357.89473684210526</v>
       </c>
-      <c r="J5" s="1">
-        <v>0.2</v>
-      </c>
+      <c r="J5"/>
       <c r="K5"/>
       <c r="L5"/>
       <c r="M5"/>
@@ -975,7 +951,7 @@
       <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -990,9 +966,7 @@
       <c r="I6" s="2">
         <v>1263.1578947368421</v>
       </c>
-      <c r="J6" s="1">
-        <v>1.2</v>
-      </c>
+      <c r="J6"/>
       <c r="K6"/>
       <c r="L6"/>
       <c r="M6"/>
@@ -1008,7 +982,7 @@
       <c r="D7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -1023,9 +997,7 @@
       <c r="I7" s="2">
         <v>421.05263157894734</v>
       </c>
-      <c r="J7" s="1">
-        <v>1.67</v>
-      </c>
+      <c r="J7"/>
       <c r="K7"/>
       <c r="L7"/>
       <c r="M7"/>
@@ -1041,7 +1013,7 @@
       <c r="D8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -1056,9 +1028,7 @@
       <c r="I8" s="2">
         <v>4105.2631578947367</v>
       </c>
-      <c r="J8" s="1">
-        <v>2.41</v>
-      </c>
+      <c r="J8"/>
       <c r="K8"/>
       <c r="L8"/>
       <c r="M8"/>
@@ -1074,7 +1044,7 @@
       <c r="D9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -1089,9 +1059,7 @@
       <c r="I9" s="2">
         <v>357.89473684210526</v>
       </c>
-      <c r="J9" s="1">
-        <v>0.21</v>
-      </c>
+      <c r="J9"/>
       <c r="K9"/>
       <c r="L9"/>
       <c r="M9"/>
@@ -1107,7 +1075,7 @@
       <c r="D10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -1122,10 +1090,8 @@
       <c r="I10" s="2">
         <v>400</v>
       </c>
-      <c r="J10" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="K10"/>
+      <c r="J10"/>
+      <c r="K10" s="3"/>
       <c r="L10"/>
       <c r="M10"/>
       <c r="N10"/>
@@ -1140,7 +1106,7 @@
       <c r="D11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F11" s="1" t="s">
@@ -1155,9 +1121,7 @@
       <c r="I11" s="2">
         <v>4378.9473684210525</v>
       </c>
-      <c r="J11" s="1">
-        <v>2.7</v>
-      </c>
+      <c r="J11"/>
       <c r="K11"/>
       <c r="L11"/>
       <c r="M11"/>
@@ -1173,7 +1137,7 @@
       <c r="D12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F12" s="1" t="s">
@@ -1188,9 +1152,7 @@
       <c r="I12" s="2">
         <v>2821.0526315789475</v>
       </c>
-      <c r="J12" s="1">
-        <v>3.12</v>
-      </c>
+      <c r="J12"/>
       <c r="K12"/>
       <c r="L12"/>
       <c r="M12"/>
@@ -1206,7 +1168,7 @@
       <c r="D13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F13" s="1" t="s">
@@ -1221,9 +1183,7 @@
       <c r="I13" s="2">
         <v>400</v>
       </c>
-      <c r="J13" s="1">
-        <v>2.71</v>
-      </c>
+      <c r="J13"/>
       <c r="K13"/>
       <c r="L13"/>
       <c r="M13"/>
@@ -1239,7 +1199,7 @@
       <c r="D14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F14" s="1" t="s">
@@ -1254,9 +1214,7 @@
       <c r="I14" s="2">
         <v>7578.9473684210525</v>
       </c>
-      <c r="J14" s="1">
-        <v>5.81</v>
-      </c>
+      <c r="J14"/>
       <c r="K14"/>
       <c r="L14"/>
       <c r="M14"/>
@@ -1272,7 +1230,7 @@
       <c r="D15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F15" s="1" t="s">
@@ -1287,9 +1245,7 @@
       <c r="I15" s="2">
         <v>3431.5789473684213</v>
       </c>
-      <c r="J15" s="1">
-        <v>5.82</v>
-      </c>
+      <c r="J15"/>
       <c r="K15"/>
       <c r="L15"/>
       <c r="M15"/>
@@ -1305,7 +1261,7 @@
       <c r="D16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F16" s="1" t="s">
@@ -1320,9 +1276,7 @@
       <c r="I16" s="2">
         <v>3536.8421052631579</v>
       </c>
-      <c r="J16" s="1">
-        <v>8.84</v>
-      </c>
+      <c r="J16"/>
       <c r="K16"/>
       <c r="L16"/>
       <c r="M16"/>
@@ -1338,7 +1292,7 @@
       <c r="D17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F17" s="1" t="s">
@@ -1353,9 +1307,7 @@
       <c r="I17" s="2">
         <v>19768.42105263158</v>
       </c>
-      <c r="J17" s="1">
-        <v>10.210000000000001</v>
-      </c>
+      <c r="J17"/>
       <c r="K17"/>
       <c r="L17"/>
       <c r="M17"/>
@@ -1371,7 +1323,7 @@
       <c r="D18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F18" s="1" t="s">
@@ -1386,9 +1338,7 @@
       <c r="I18" s="2">
         <v>6252.6315789473683</v>
       </c>
-      <c r="J18" s="1">
-        <v>14.14</v>
-      </c>
+      <c r="J18"/>
       <c r="K18"/>
       <c r="L18"/>
       <c r="M18"/>
@@ -1404,7 +1354,7 @@
       <c r="D19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F19" s="1" t="s">
@@ -1419,9 +1369,7 @@
       <c r="I19" s="2">
         <v>11873.684210526315</v>
       </c>
-      <c r="J19" s="1">
-        <v>28.2</v>
-      </c>
+      <c r="J19"/>
       <c r="K19"/>
       <c r="L19"/>
       <c r="M19"/>
@@ -1437,7 +1385,7 @@
       <c r="D20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F20" s="1" t="s">
@@ -1452,9 +1400,7 @@
       <c r="I20" s="2">
         <v>2526.3157894736842</v>
       </c>
-      <c r="J20" s="1">
-        <v>0.1</v>
-      </c>
+      <c r="J20"/>
       <c r="K20"/>
       <c r="L20"/>
       <c r="M20"/>
@@ -1470,7 +1416,7 @@
       <c r="D21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F21" s="1" t="s">
@@ -1485,9 +1431,7 @@
       <c r="I21" s="2">
         <v>3894.7368421052633</v>
       </c>
-      <c r="J21" s="1">
-        <v>8.41</v>
-      </c>
+      <c r="J21"/>
       <c r="K21"/>
       <c r="L21"/>
       <c r="M21"/>
@@ -1503,7 +1447,7 @@
       <c r="D22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F22" s="1" t="s">
@@ -1518,9 +1462,7 @@
       <c r="I22" s="2">
         <v>30736.842105263157</v>
       </c>
-      <c r="J22" s="1">
-        <v>30.42</v>
-      </c>
+      <c r="J22"/>
       <c r="K22"/>
       <c r="L22"/>
       <c r="M22"/>
@@ -1536,7 +1478,7 @@
       <c r="D23" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F23" s="1" t="s">
@@ -1551,9 +1493,7 @@
       <c r="I23" s="2">
         <v>15284.21052631579</v>
       </c>
-      <c r="J23" s="1">
-        <v>23.42</v>
-      </c>
+      <c r="J23"/>
       <c r="K23"/>
       <c r="L23"/>
       <c r="M23"/>
@@ -1569,7 +1509,7 @@
       <c r="D24" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F24" s="1" t="s">
@@ -1584,9 +1524,7 @@
       <c r="I24" s="2">
         <v>11347.368421052632</v>
       </c>
-      <c r="J24" s="1">
-        <v>44.92</v>
-      </c>
+      <c r="J24"/>
       <c r="K24"/>
       <c r="L24"/>
       <c r="M24"/>
@@ -1602,7 +1540,7 @@
       <c r="D25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F25" s="1" t="s">
@@ -1617,9 +1555,7 @@
       <c r="I25" s="2">
         <v>18315.78947368421</v>
       </c>
-      <c r="J25" s="1">
-        <v>41.43</v>
-      </c>
+      <c r="J25"/>
       <c r="K25"/>
       <c r="L25"/>
       <c r="M25"/>
@@ -1635,7 +1571,7 @@
       <c r="D26" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F26" s="1" t="s">
@@ -1650,9 +1586,7 @@
       <c r="I26" s="2">
         <v>61600</v>
       </c>
-      <c r="J26" s="1">
-        <v>77</v>
-      </c>
+      <c r="J26"/>
       <c r="K26"/>
       <c r="L26"/>
       <c r="M26"/>
@@ -1668,7 +1602,7 @@
       <c r="D27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F27" s="1" t="s">
@@ -1683,9 +1617,7 @@
       <c r="I27" s="2">
         <v>59284.210526315786</v>
       </c>
-      <c r="J27" s="1">
-        <v>59.91</v>
-      </c>
+      <c r="J27"/>
       <c r="K27"/>
       <c r="L27"/>
       <c r="M27"/>
@@ -1701,7 +1633,7 @@
       <c r="D28" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F28" s="1" t="s">
@@ -1716,9 +1648,7 @@
       <c r="I28" s="2">
         <v>44442.105263157893</v>
       </c>
-      <c r="J28" s="1">
-        <v>44.91</v>
-      </c>
+      <c r="J28"/>
       <c r="K28"/>
       <c r="L28"/>
       <c r="M28"/>
@@ -1734,7 +1664,7 @@
       <c r="D29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F29" s="1" t="s">
@@ -1749,9 +1679,7 @@
       <c r="I29" s="2">
         <v>33978.947368421053</v>
       </c>
-      <c r="J29" s="1">
-        <v>48.91</v>
-      </c>
+      <c r="J29"/>
       <c r="K29"/>
       <c r="L29"/>
       <c r="M29"/>
@@ -1767,7 +1695,7 @@
       <c r="D30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E30" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F30" s="1" t="s">
@@ -1782,9 +1710,7 @@
       <c r="I30" s="2">
         <v>30568.42105263158</v>
       </c>
-      <c r="J30" s="1">
-        <v>90.75</v>
-      </c>
+      <c r="J30"/>
       <c r="K30"/>
       <c r="L30"/>
       <c r="M30"/>
@@ -1800,7 +1726,7 @@
       <c r="D31" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F31" s="1" t="s">
@@ -1815,9 +1741,7 @@
       <c r="I31" s="2">
         <v>26484.21052631579</v>
       </c>
-      <c r="J31" s="1">
-        <v>74</v>
-      </c>
+      <c r="J31"/>
       <c r="K31"/>
       <c r="L31"/>
       <c r="M31"/>
@@ -1833,7 +1757,7 @@
       <c r="D32" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F32" s="1" t="s">
@@ -1848,9 +1772,7 @@
       <c r="I32" s="2">
         <v>26400</v>
       </c>
-      <c r="J32" s="1">
-        <v>22</v>
-      </c>
+      <c r="J32"/>
       <c r="K32"/>
       <c r="L32"/>
       <c r="M32"/>
@@ -1866,7 +1788,7 @@
       <c r="D33" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F33" s="1" t="s">
@@ -1881,9 +1803,7 @@
       <c r="I33" s="2">
         <v>28252.63157894737</v>
       </c>
-      <c r="J33" s="1">
-        <v>22</v>
-      </c>
+      <c r="J33"/>
       <c r="K33"/>
       <c r="L33"/>
       <c r="M33"/>
@@ -1899,7 +1819,7 @@
       <c r="D34" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F34" s="1" t="s">
@@ -1914,9 +1834,7 @@
       <c r="I34" s="2">
         <v>631.57894736842104</v>
       </c>
-      <c r="J34" s="1">
-        <v>1</v>
-      </c>
+      <c r="J34"/>
       <c r="K34"/>
       <c r="L34"/>
       <c r="M34"/>
@@ -1932,7 +1850,7 @@
       <c r="D35" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E35" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F35" s="1" t="s">
@@ -1947,9 +1865,7 @@
       <c r="I35" s="2">
         <v>1094.7368421052631</v>
       </c>
-      <c r="J35" s="1">
-        <v>1.3</v>
-      </c>
+      <c r="J35"/>
       <c r="K35"/>
       <c r="L35"/>
       <c r="M35"/>
@@ -1965,7 +1881,7 @@
       <c r="D36" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E36" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F36" s="1" t="s">
@@ -1980,9 +1896,7 @@
       <c r="I36" s="2">
         <v>2315.7894736842104</v>
       </c>
-      <c r="J36" s="1">
-        <v>1.51</v>
-      </c>
+      <c r="J36"/>
       <c r="K36"/>
       <c r="L36"/>
       <c r="M36"/>
@@ -1998,7 +1912,7 @@
       <c r="D37" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E37" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F37" s="1" t="s">
@@ -2013,9 +1927,7 @@
       <c r="I37" s="2">
         <v>2589.4736842105262</v>
       </c>
-      <c r="J37" s="1">
-        <v>3.62</v>
-      </c>
+      <c r="J37"/>
       <c r="K37"/>
       <c r="L37"/>
       <c r="M37"/>
@@ -2031,7 +1943,7 @@
       <c r="D38" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E38" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F38" s="1" t="s">
@@ -2046,9 +1958,7 @@
       <c r="I38" s="2">
         <v>484.21052631578948</v>
       </c>
-      <c r="J38" s="1">
-        <v>5.75</v>
-      </c>
+      <c r="J38"/>
       <c r="K38"/>
       <c r="L38"/>
       <c r="M38"/>
@@ -2056,11 +1966,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B38">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
tabla excel arreglo campo description
</commit_message>
<xml_diff>
--- a/seeders/Table_Budget.xlsx
+++ b/seeders/Table_Budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GitHub\do_and_check_back2\seeders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F5A1B4-AA67-489B-B730-C0A338697463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E9D029-323F-487E-8F09-CEBD5424CD1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{78331709-7AEC-4852-8807-FA6C03489801}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="56">
   <si>
     <t>code</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>totalLabourCost</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -242,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -251,11 +254,59 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -387,51 +438,6 @@
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -450,14 +456,14 @@
   <autoFilter ref="A1:I38" xr:uid="{73859FA6-B201-4B3E-AA95-B0103745529F}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{02AB9CA0-F38A-4F84-B089-91407259440B}" name="code" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{28BAAC49-883E-4794-B5A9-A36102880638}" name="title" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{45D60C40-648C-4915-8246-855E6240C002}" name="description" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{1A487E48-40EA-4B23-A821-233B479E0007}" name="taskGroup" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{50E1C117-0C18-4F8C-8E11-8574C6A6DF81}" name="taskStatus" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{604AAADE-9C9E-4848-AD83-955E0F214682}" name="unit" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{0C826A12-79CF-4C51-AE86-631B484247B9}" name="totalBudgetQty" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{292D0ECB-729B-472C-B2BB-C538B430EE2E}" name="totalBudgetHrs" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{42B9CA9F-909E-4799-B73A-EE7BE06E26CD}" name="totalLabourCost" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{28BAAC49-883E-4794-B5A9-A36102880638}" name="title" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{45D60C40-648C-4915-8246-855E6240C002}" name="description" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{1A487E48-40EA-4B23-A821-233B479E0007}" name="taskGroup" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{50E1C117-0C18-4F8C-8E11-8574C6A6DF81}" name="taskStatus" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{604AAADE-9C9E-4848-AD83-955E0F214682}" name="unit" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{0C826A12-79CF-4C51-AE86-631B484247B9}" name="totalBudgetQty" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{292D0ECB-729B-472C-B2BB-C538B430EE2E}" name="totalBudgetHrs" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{42B9CA9F-909E-4799-B73A-EE7BE06E26CD}" name="totalLabourCost" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -763,7 +769,7 @@
   <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="C2" sqref="C2:C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -824,6 +830,9 @@
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C2" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
@@ -855,6 +864,9 @@
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C3" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
@@ -886,6 +898,9 @@
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C4" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
@@ -917,6 +932,9 @@
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C5" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
@@ -948,6 +966,9 @@
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="C6" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
@@ -979,6 +1000,9 @@
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="C7" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1010,6 +1034,9 @@
       <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="C8" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1041,6 +1068,9 @@
       <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="C9" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1072,6 +1102,9 @@
       <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C10" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D10" s="1" t="s">
         <v>5</v>
       </c>
@@ -1103,6 +1136,9 @@
       <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="C11" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D11" s="1" t="s">
         <v>17</v>
       </c>
@@ -1134,6 +1170,9 @@
       <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="C12" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D12" s="1" t="s">
         <v>17</v>
       </c>
@@ -1165,6 +1204,9 @@
       <c r="B13" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="C13" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D13" s="1" t="s">
         <v>17</v>
       </c>
@@ -1196,6 +1238,9 @@
       <c r="B14" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="C14" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D14" s="1" t="s">
         <v>17</v>
       </c>
@@ -1227,6 +1272,9 @@
       <c r="B15" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="C15" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D15" s="1" t="s">
         <v>17</v>
       </c>
@@ -1258,6 +1306,9 @@
       <c r="B16" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="C16" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D16" s="1" t="s">
         <v>17</v>
       </c>
@@ -1289,6 +1340,9 @@
       <c r="B17" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="C17" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1320,6 +1374,9 @@
       <c r="B18" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="C18" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1351,6 +1408,9 @@
       <c r="B19" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="C19" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D19" s="1" t="s">
         <v>17</v>
       </c>
@@ -1382,6 +1442,9 @@
       <c r="B20" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="C20" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D20" s="1" t="s">
         <v>25</v>
       </c>
@@ -1413,6 +1476,9 @@
       <c r="B21" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="C21" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D21" s="1" t="s">
         <v>27</v>
       </c>
@@ -1444,6 +1510,9 @@
       <c r="B22" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="C22" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D22" s="1" t="s">
         <v>27</v>
       </c>
@@ -1475,6 +1544,9 @@
       <c r="B23" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="C23" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D23" s="1" t="s">
         <v>27</v>
       </c>
@@ -1506,6 +1578,9 @@
       <c r="B24" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="C24" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D24" s="1" t="s">
         <v>27</v>
       </c>
@@ -1537,6 +1612,9 @@
       <c r="B25" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="C25" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D25" s="1" t="s">
         <v>27</v>
       </c>
@@ -1568,6 +1646,9 @@
       <c r="B26" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="C26" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D26" s="1" t="s">
         <v>27</v>
       </c>
@@ -1599,6 +1680,9 @@
       <c r="B27" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="C27" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D27" s="1" t="s">
         <v>27</v>
       </c>
@@ -1630,6 +1714,9 @@
       <c r="B28" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="C28" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D28" s="1" t="s">
         <v>27</v>
       </c>
@@ -1661,6 +1748,9 @@
       <c r="B29" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="C29" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D29" s="1" t="s">
         <v>27</v>
       </c>
@@ -1692,6 +1782,9 @@
       <c r="B30" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="C30" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D30" s="1" t="s">
         <v>27</v>
       </c>
@@ -1723,6 +1816,9 @@
       <c r="B31" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="C31" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D31" s="1" t="s">
         <v>27</v>
       </c>
@@ -1754,6 +1850,9 @@
       <c r="B32" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="C32" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D32" s="1" t="s">
         <v>27</v>
       </c>
@@ -1785,6 +1884,9 @@
       <c r="B33" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="C33" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D33" s="1" t="s">
         <v>27</v>
       </c>
@@ -1816,6 +1918,9 @@
       <c r="B34" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="C34" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D34" s="1" t="s">
         <v>42</v>
       </c>
@@ -1847,6 +1952,9 @@
       <c r="B35" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="C35" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D35" s="1" t="s">
         <v>42</v>
       </c>
@@ -1878,6 +1986,9 @@
       <c r="B36" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="C36" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D36" s="1" t="s">
         <v>42</v>
       </c>
@@ -1909,6 +2020,9 @@
       <c r="B37" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="C37" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D37" s="1" t="s">
         <v>42</v>
       </c>
@@ -1940,6 +2054,9 @@
       <c r="B38" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="C38" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D38" s="1" t="s">
         <v>42</v>
       </c>
@@ -1966,7 +2083,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B38">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>